<commit_message>
updating the bedload stuff for the paper
still need to add onto the supplementary materials tho
</commit_message>
<xml_diff>
--- a/Bedload/bedloadGSDs.xlsx
+++ b/Bedload/bedloadGSDs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Bedload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E844C8A9-4B6C-4353-AFAB-930E296ABBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5D1DE1-C942-4A43-90C6-9DD7E5723F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sediment" sheetId="1" r:id="rId1"/>
-    <sheet name="Wood Debris" sheetId="2" r:id="rId2"/>
+    <sheet name="Final" sheetId="3" r:id="rId1"/>
+    <sheet name="Sediment" sheetId="1" r:id="rId2"/>
+    <sheet name="Wood Debris" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>pan</t>
   </si>
@@ -76,13 +77,47 @@
   </si>
   <si>
     <t>TOTAL (%)</t>
+  </si>
+  <si>
+    <t>Total mass from the sieves</t>
+  </si>
+  <si>
+    <t>Size (mm)</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>total (kg)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +125,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +165,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -125,11 +180,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,7 +279,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,19 +609,476 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699A0717-E7CB-4E57-A578-ABA98CA0B5D1}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>11.2</v>
+      </c>
+      <c r="B3" s="14">
+        <v>4</v>
+      </c>
+      <c r="C3" s="15">
+        <v>24.492999999999999</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0</v>
+      </c>
+      <c r="E3" s="16">
+        <v>0</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16">
+        <v>0</v>
+      </c>
+      <c r="I3" s="16">
+        <v>0</v>
+      </c>
+      <c r="J3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>8</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>10.259</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+      <c r="G4" s="16">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15">
+        <v>0.996</v>
+      </c>
+      <c r="J4" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>5.6</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>17.54</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1.0137</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="I5" s="15">
+        <v>1.036</v>
+      </c>
+      <c r="J5" s="19">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1.0545</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1.5669999999999999</v>
+      </c>
+      <c r="J6" s="19">
+        <v>0.56530000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>2.8</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15">
+        <v>14.249000000000001</v>
+      </c>
+      <c r="D7" s="15">
+        <v>2.7E-2</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="F7" s="20">
+        <v>1.5296000000000001</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0.1007</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0.63829999999999998</v>
+      </c>
+      <c r="I7" s="21">
+        <v>3.94</v>
+      </c>
+      <c r="J7" s="19">
+        <v>0.77400000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>2</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15">
+        <v>13.52</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.128</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.68830000000000002</v>
+      </c>
+      <c r="F8" s="15">
+        <v>2.3923999999999999</v>
+      </c>
+      <c r="G8" s="15">
+        <v>8.5199999999999998E-2</v>
+      </c>
+      <c r="H8" s="15">
+        <v>1.3906000000000001</v>
+      </c>
+      <c r="I8" s="21">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0.435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>1.4</v>
+      </c>
+      <c r="B9" s="22">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="C9" s="15">
+        <v>13.35</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.31419999999999998</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="F9" s="15">
+        <v>3.5289000000000001</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="H9" s="15">
+        <v>2.9470000000000001</v>
+      </c>
+      <c r="I9" s="21">
+        <v>4.7329999999999997</v>
+      </c>
+      <c r="J9" s="19">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>1</v>
+      </c>
+      <c r="B10" s="22">
+        <v>0.70120000000000005</v>
+      </c>
+      <c r="C10" s="15">
+        <v>9.56</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1.4064000000000001</v>
+      </c>
+      <c r="F10" s="15">
+        <v>3.9658000000000002</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0.43219999999999997</v>
+      </c>
+      <c r="H10" s="15">
+        <v>5.306</v>
+      </c>
+      <c r="I10" s="21">
+        <v>4.13</v>
+      </c>
+      <c r="J10" s="19">
+        <v>0.69030000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="B11" s="22">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="C11" s="15">
+        <v>8.0239999999999991</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0.83</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1.9267000000000001</v>
+      </c>
+      <c r="F11" s="15">
+        <v>4.3182</v>
+      </c>
+      <c r="G11" s="15">
+        <v>1.42</v>
+      </c>
+      <c r="H11" s="15">
+        <v>8.6374999999999993</v>
+      </c>
+      <c r="I11" s="21">
+        <v>3.8551000000000002</v>
+      </c>
+      <c r="J11" s="19">
+        <v>0.74650000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="B12" s="22">
+        <v>1.0680000000000001</v>
+      </c>
+      <c r="C12" s="15">
+        <v>6.02</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1.2862</v>
+      </c>
+      <c r="E12" s="15">
+        <v>1.8748</v>
+      </c>
+      <c r="F12" s="15">
+        <v>3.956</v>
+      </c>
+      <c r="G12" s="15">
+        <v>1.4590000000000001</v>
+      </c>
+      <c r="H12" s="15">
+        <v>11.17</v>
+      </c>
+      <c r="I12" s="15">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="J12" s="19">
+        <v>0.72140000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="22">
+        <v>2.7709999999999999</v>
+      </c>
+      <c r="C13" s="15">
+        <v>9.1370000000000005</v>
+      </c>
+      <c r="D13" s="15">
+        <v>4.6239999999999997</v>
+      </c>
+      <c r="E13" s="15">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="F13" s="15">
+        <v>4.9240000000000004</v>
+      </c>
+      <c r="G13" s="15">
+        <v>10.197100000000001</v>
+      </c>
+      <c r="H13" s="15">
+        <v>22.088999999999999</v>
+      </c>
+      <c r="I13" s="15">
+        <v>2.2869999999999999</v>
+      </c>
+      <c r="J13" s="19">
+        <v>1.1431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="23">
+        <f>SUM(B3:B13)/1000</f>
+        <v>9.9492000000000018E-3</v>
+      </c>
+      <c r="C14" s="24">
+        <f>SUM(C3:C13)/1000</f>
+        <v>0.14232199999999998</v>
+      </c>
+      <c r="D14" s="24">
+        <f t="shared" ref="D14:J14" si="0">SUM(D3:D13)/1000</f>
+        <v>7.6644E-3</v>
+      </c>
+      <c r="E14" s="24">
+        <f t="shared" si="0"/>
+        <v>1.0039200000000002E-2</v>
+      </c>
+      <c r="F14" s="24">
+        <f t="shared" si="0"/>
+        <v>2.6683100000000001E-2</v>
+      </c>
+      <c r="G14" s="24">
+        <f t="shared" si="0"/>
+        <v>1.41662E-2</v>
+      </c>
+      <c r="H14" s="24">
+        <f>SUM(H3:H13)/1000</f>
+        <v>5.37464E-2</v>
+      </c>
+      <c r="I14" s="24">
+        <f t="shared" si="0"/>
+        <v>2.2711099999999998E-2</v>
+      </c>
+      <c r="J14" s="24">
+        <f t="shared" si="0"/>
+        <v>6.2585999999999996E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -452,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>11.2</v>
       </c>
@@ -464,7 +1104,7 @@
         <v>24.492999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -476,7 +1116,7 @@
         <v>10.259</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5.6</v>
       </c>
@@ -488,7 +1128,7 @@
         <v>17.543800000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -500,7 +1140,7 @@
         <v>16.167000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2.8</v>
       </c>
@@ -512,7 +1152,7 @@
         <v>14.247999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -524,7 +1164,7 @@
         <v>13.518000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -533,7 +1173,7 @@
         <v>0.56200000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -542,7 +1182,7 @@
         <v>0.70120000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.71</v>
       </c>
@@ -550,7 +1190,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.5</v>
       </c>
@@ -559,7 +1199,7 @@
         <v>1.0680000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.25</v>
       </c>
@@ -570,7 +1210,7 @@
         <v>9.1370000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +1222,7 @@
         <v>1.9748000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -598,7 +1238,7 @@
         <v>107.34060000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -612,12 +1252,12 @@
         <v>120.92940000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -628,13 +1268,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>11.2</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="6">
-        <f>C3/$C$15</f>
+        <f t="shared" ref="C20:C32" si="0">C3/$C$15</f>
         <v>0.35973811065544281</v>
       </c>
       <c r="D20" s="6">
@@ -642,166 +1282,166 @@
         <v>0.22818020394892516</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>8</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="6">
-        <f>C4/$C$15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D21" s="6">
-        <f t="shared" ref="D21:D31" si="0">D4/$D$15</f>
+        <f t="shared" ref="D21:D31" si="1">D4/$D$15</f>
         <v>9.5574274785123245E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>5.6</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="6">
-        <f>C5/$C$15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D22" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1634404875694751</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>4</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="6">
-        <f>C6/$C$15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D23" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1506140267522261</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>2.8</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="6">
-        <f>C7/$C$15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13273635511633061</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>2</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="6">
-        <f>C8/$C$15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D25" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1259355733059066</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>1.4</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="4">
-        <f>C9/$C$15</f>
+        <f t="shared" si="0"/>
         <v>5.0543204547089722E-2</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>1</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="4">
-        <f>C10/$C$15</f>
+        <f t="shared" si="0"/>
         <v>6.3062090797899123E-2</v>
       </c>
       <c r="D27" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>0.71</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="4">
-        <f>C11/$C$15</f>
+        <f t="shared" si="0"/>
         <v>7.6174544931290014E-2</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>0.5</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="4">
-        <f>C12/$C$15</f>
+        <f t="shared" si="0"/>
         <v>9.6050075545003236E-2</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>0.25</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="4">
-        <f>C13/$C$15</f>
+        <f t="shared" si="0"/>
         <v>0.249208576156558</v>
       </c>
       <c r="D30" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.5121566303896196E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="2">
-        <f>C14/$C$15</f>
+        <f t="shared" si="0"/>
         <v>0.10522339736671701</v>
       </c>
       <c r="D31" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8397512218116911E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="1">
-        <f>C15/$C$15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D32" s="1">
@@ -809,11 +1449,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="8"/>
       <c r="C34" s="1">
         <f>SUM(C20:C25)</f>
         <v>0.35973811065544281</v>
@@ -827,11 +1466,10 @@
         <v>0.62810951606671472</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="8"/>
       <c r="C35" s="1">
         <f>SUM(C26:C30)</f>
         <v>0.53503849197784015</v>
@@ -845,11 +1483,10 @@
         <v>0.31008002914086819</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="8"/>
       <c r="C36" s="1">
         <f>SUM(C31)</f>
         <v>0.10522339736671701</v>
@@ -863,7 +1500,7 @@
         <v>6.1810454792416966E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <f>SUM(C34:C36)</f>
         <v>1</v>
@@ -873,12 +1510,12 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -889,7 +1526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>11.2</v>
       </c>
@@ -899,113 +1536,113 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>8</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="6">
-        <f>C21+C40</f>
+        <f t="shared" ref="C41:C51" si="2">C21+C40</f>
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>5.6</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="6">
-        <f>C22+C41</f>
+        <f t="shared" si="2"/>
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>4</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="6">
-        <f>C23+C42</f>
+        <f t="shared" si="2"/>
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>2.8</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="6">
-        <f>C24+C43</f>
+        <f t="shared" si="2"/>
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>2</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="6">
-        <f>C25+C44</f>
+        <f t="shared" si="2"/>
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>1.4</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="4">
-        <f>C26+C45</f>
+        <f t="shared" si="2"/>
         <v>0.41028131520253253</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>1</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4">
-        <f>C27+C46</f>
+        <f t="shared" si="2"/>
         <v>0.47334340600043168</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>0.71</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="4">
-        <f>C28+C47</f>
+        <f t="shared" si="2"/>
         <v>0.54951795093172173</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>0.5</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="4">
-        <f>C29+C48</f>
+        <f t="shared" si="2"/>
         <v>0.64556802647672495</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>0.25</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="4">
-        <f>C30+C49</f>
+        <f t="shared" si="2"/>
         <v>0.89477660263328296</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="2">
-        <f>C31+C50</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1014,7 +1651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFEEC62-4264-4E95-A17A-D4E215EDD374}">
   <dimension ref="A2:D15"/>
   <sheetViews>
@@ -1022,12 +1659,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1041,7 +1678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>11.2</v>
       </c>
@@ -1055,7 +1692,7 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -1067,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5.6</v>
       </c>
@@ -1079,7 +1716,7 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1091,7 +1728,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2.8</v>
       </c>
@@ -1103,7 +1740,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -1115,7 +1752,7 @@
         <v>0.50700000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -1127,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1139,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.71</v>
       </c>
@@ -1150,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.5</v>
       </c>
@@ -1162,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.25</v>
       </c>
@@ -1173,7 +1810,7 @@
         <v>9.1370000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1822,7 @@
         <v>1.9748000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
updating bedload stuff for paper
</commit_message>
<xml_diff>
--- a/Bedload/bedloadGSDs.xlsx
+++ b/Bedload/bedloadGSDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Bedload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5D1DE1-C942-4A43-90C6-9DD7E5723F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06C5613-8636-4475-9850-132058BFF747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>pan</t>
   </si>
@@ -107,6 +107,39 @@
   </si>
   <si>
     <t>total (kg)</t>
+  </si>
+  <si>
+    <t>Percentage of each grain size</t>
+  </si>
+  <si>
+    <t>total (g)</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Percentage of each grain size class</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Gravel  &gt;2mm</t>
+  </si>
+  <si>
+    <t>Fines (&lt;0.2mm)</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -172,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -258,11 +291,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,55 +321,82 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -610,456 +679,1363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699A0717-E7CB-4E57-A578-ABA98CA0B5D1}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
         <v>11.2</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>4</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="13">
         <v>24.492999999999999</v>
       </c>
-      <c r="D3" s="16">
-        <v>0</v>
-      </c>
-      <c r="E3" s="16">
-        <v>0</v>
-      </c>
-      <c r="F3" s="16">
-        <v>0</v>
-      </c>
-      <c r="G3" s="16">
-        <v>0</v>
-      </c>
-      <c r="H3" s="16">
-        <v>0</v>
-      </c>
-      <c r="I3" s="16">
-        <v>0</v>
-      </c>
-      <c r="J3" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
         <v>8</v>
       </c>
-      <c r="B4" s="14">
-        <v>0</v>
-      </c>
-      <c r="C4" s="15">
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13">
         <v>10.259</v>
       </c>
-      <c r="D4" s="16">
-        <v>0</v>
-      </c>
-      <c r="E4" s="16">
-        <v>0</v>
-      </c>
-      <c r="F4" s="16">
-        <v>0</v>
-      </c>
-      <c r="G4" s="16">
-        <v>0</v>
-      </c>
-      <c r="H4" s="16">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
         <v>0.996</v>
       </c>
-      <c r="J4" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="J4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
         <v>5.6</v>
       </c>
-      <c r="B5" s="14">
-        <v>0</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="B5" s="12">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
         <v>17.54</v>
       </c>
-      <c r="D5" s="16">
-        <v>0</v>
-      </c>
-      <c r="E5" s="16">
-        <v>0</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
         <v>1.0137</v>
       </c>
-      <c r="G5" s="16">
-        <v>0</v>
-      </c>
-      <c r="H5" s="15">
+      <c r="G5" s="14">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
         <v>0.97299999999999998</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="13">
         <v>1.036</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="17">
         <v>0.29499999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
-      <c r="B6" s="14">
-        <v>0</v>
-      </c>
-      <c r="C6" s="15">
+      <c r="B6" s="12">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
         <v>16.170000000000002</v>
       </c>
-      <c r="D6" s="16">
-        <v>0</v>
-      </c>
-      <c r="E6" s="16">
-        <v>0</v>
-      </c>
-      <c r="F6" s="15">
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
         <v>1.0545</v>
       </c>
-      <c r="G6" s="16">
-        <v>0</v>
-      </c>
-      <c r="H6" s="15">
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
         <v>0.59499999999999997</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="13">
         <v>1.5669999999999999</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="17">
         <v>0.56530000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
         <v>2.8</v>
       </c>
-      <c r="B7" s="14">
-        <v>0</v>
-      </c>
-      <c r="C7" s="15">
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
         <v>14.249000000000001</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>2.7E-2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="13">
         <v>0.90300000000000002</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="18">
         <v>1.5296000000000001</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <v>0.1007</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="13">
         <v>0.63829999999999998</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="19">
         <v>3.94</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="17">
         <v>0.77400000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
         <v>2</v>
       </c>
-      <c r="B8" s="14">
-        <v>0</v>
-      </c>
-      <c r="C8" s="15">
+      <c r="B8" s="12">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13">
         <v>13.52</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <v>0.128</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="13">
         <v>0.68830000000000002</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <v>2.3923999999999999</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>8.5199999999999998E-2</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="13">
         <v>1.3906000000000001</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="19">
         <v>0.14599999999999999</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="17">
         <v>0.435</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
         <v>1.4</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>0.56200000000000006</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="13">
         <v>13.35</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="13">
         <v>0.31419999999999998</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="13">
         <v>1.02</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="13">
         <v>3.5289000000000001</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="13">
         <v>0.47199999999999998</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="13">
         <v>2.9470000000000001</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="19">
         <v>4.7329999999999997</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="17">
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
         <v>1</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>0.70120000000000005</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="13">
         <v>9.56</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="13">
         <v>0.45500000000000002</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="13">
         <v>1.4064000000000001</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="13">
         <v>3.9658000000000002</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="13">
         <v>0.43219999999999997</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="13">
         <v>5.306</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="19">
         <v>4.13</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="17">
         <v>0.69030000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
         <v>0.7</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>0.84699999999999998</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <v>8.0239999999999991</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="13">
         <v>0.83</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="13">
         <v>1.9267000000000001</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="13">
         <v>4.3182</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="13">
         <v>1.42</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="13">
         <v>8.6374999999999993</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="19">
         <v>3.8551000000000002</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="17">
         <v>0.74650000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
         <v>0.5</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="20">
         <v>1.0680000000000001</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="13">
         <v>6.02</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="13">
         <v>1.2862</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="13">
         <v>1.8748</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="13">
         <v>3.956</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="13">
         <v>1.4590000000000001</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="13">
         <v>11.17</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="13">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="17">
         <v>0.72140000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="22">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="20">
         <v>2.7709999999999999</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="13">
         <v>9.1370000000000005</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="13">
         <v>4.6239999999999997</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="13">
         <v>2.2200000000000002</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="13">
         <v>4.9240000000000004</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="13">
         <v>10.197100000000001</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="13">
         <v>22.088999999999999</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="13">
         <v>2.2869999999999999</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="17">
         <v>1.1431</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1">
+        <f>SUM(B3:B13)</f>
+        <v>9.9492000000000012</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:J14" si="0">SUM(C3:C13)</f>
+        <v>142.32199999999997</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>7.6643999999999997</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>10.039200000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>26.6831</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>14.1662</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>53.746400000000001</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>22.711099999999998</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2585999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B15" s="21">
         <f>SUM(B3:B13)/1000</f>
         <v>9.9492000000000018E-3</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C15" s="22">
         <f>SUM(C3:C13)/1000</f>
         <v>0.14232199999999998</v>
       </c>
-      <c r="D14" s="24">
-        <f t="shared" ref="D14:J14" si="0">SUM(D3:D13)/1000</f>
+      <c r="D15" s="22">
+        <f>SUM(D3:D13)/1000</f>
         <v>7.6644E-3</v>
       </c>
-      <c r="E14" s="24">
-        <f t="shared" si="0"/>
+      <c r="E15" s="22">
+        <f>SUM(E3:E13)/1000</f>
         <v>1.0039200000000002E-2</v>
       </c>
-      <c r="F14" s="24">
-        <f t="shared" si="0"/>
+      <c r="F15" s="22">
+        <f>SUM(F3:F13)/1000</f>
         <v>2.6683100000000001E-2</v>
       </c>
-      <c r="G14" s="24">
-        <f t="shared" si="0"/>
+      <c r="G15" s="22">
+        <f>SUM(G3:G13)/1000</f>
         <v>1.41662E-2</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H15" s="22">
         <f>SUM(H3:H13)/1000</f>
         <v>5.37464E-2</v>
       </c>
-      <c r="I14" s="24">
-        <f t="shared" si="0"/>
+      <c r="I15" s="22">
+        <f>SUM(I3:I13)/1000</f>
         <v>2.2711099999999998E-2</v>
       </c>
-      <c r="J14" s="24">
-        <f t="shared" si="0"/>
+      <c r="J15" s="22">
+        <f>SUM(J3:J13)/1000</f>
         <v>6.2585999999999996E-3</v>
       </c>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>11.2</v>
+      </c>
+      <c r="B19" s="28">
+        <f>B3/B$14</f>
+        <v>0.402042375266353</v>
+      </c>
+      <c r="C19" s="28">
+        <f t="shared" ref="C19:J19" si="1">C3/C$14</f>
+        <v>0.17209567038124818</v>
+      </c>
+      <c r="D19" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>8</v>
+      </c>
+      <c r="B20" s="28">
+        <f>B4/B$14</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="28">
+        <f t="shared" ref="C20:J20" si="2">C4/C$14</f>
+        <v>7.2083023004173644E-2</v>
+      </c>
+      <c r="D20" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="28">
+        <f t="shared" si="2"/>
+        <v>4.3855207365561338E-2</v>
+      </c>
+      <c r="J20" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>5.6</v>
+      </c>
+      <c r="B21" s="28">
+        <f t="shared" ref="B20:J30" si="3">B5/B$14</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="28">
+        <f t="shared" si="3"/>
+        <v>0.12324166327061173</v>
+      </c>
+      <c r="D21" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="28">
+        <f t="shared" si="3"/>
+        <v>3.7990338453927769E-2</v>
+      </c>
+      <c r="G21" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="28">
+        <f t="shared" si="3"/>
+        <v>1.8103538097435361E-2</v>
+      </c>
+      <c r="I21" s="28">
+        <f t="shared" si="3"/>
+        <v>4.561646067341521E-2</v>
+      </c>
+      <c r="J21" s="28">
+        <f t="shared" si="3"/>
+        <v>4.7135142044546705E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>4</v>
+      </c>
+      <c r="B22" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C22" s="28">
+        <f t="shared" si="3"/>
+        <v>0.11361560405278175</v>
+      </c>
+      <c r="D22" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="28">
+        <f t="shared" si="3"/>
+        <v>3.9519396172108937E-2</v>
+      </c>
+      <c r="G22" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="28">
+        <f t="shared" si="3"/>
+        <v>1.1070508908503638E-2</v>
+      </c>
+      <c r="I22" s="28">
+        <f t="shared" si="3"/>
+        <v>6.8997098335175311E-2</v>
+      </c>
+      <c r="J22" s="28">
+        <f t="shared" si="3"/>
+        <v>9.0323714568753405E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="B23" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C23" s="28">
+        <f t="shared" si="3"/>
+        <v>0.10011804218602889</v>
+      </c>
+      <c r="D23" s="28">
+        <f t="shared" si="3"/>
+        <v>3.5227806481916393E-3</v>
+      </c>
+      <c r="E23" s="28">
+        <f t="shared" si="3"/>
+        <v>8.9947406167822125E-2</v>
+      </c>
+      <c r="F23" s="28">
+        <f t="shared" si="3"/>
+        <v>5.7324673669850959E-2</v>
+      </c>
+      <c r="G23" s="28">
+        <f t="shared" si="3"/>
+        <v>7.1084694554644154E-3</v>
+      </c>
+      <c r="H23" s="28">
+        <f t="shared" si="3"/>
+        <v>1.18761442626855E-2</v>
+      </c>
+      <c r="I23" s="28">
+        <f t="shared" si="3"/>
+        <v>0.17348345082360608</v>
+      </c>
+      <c r="J23" s="28">
+        <f t="shared" si="3"/>
+        <v>0.12366983031348865</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>2</v>
+      </c>
+      <c r="B24" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C24" s="29">
+        <f t="shared" si="3"/>
+        <v>9.499585447084781E-2</v>
+      </c>
+      <c r="D24" s="29">
+        <f t="shared" si="3"/>
+        <v>1.6700589739575181E-2</v>
+      </c>
+      <c r="E24" s="29">
+        <f t="shared" si="3"/>
+        <v>6.8561239939437399E-2</v>
+      </c>
+      <c r="F24" s="29">
+        <f t="shared" si="3"/>
+        <v>8.9659747180799831E-2</v>
+      </c>
+      <c r="G24" s="29">
+        <f t="shared" si="3"/>
+        <v>6.0143157656958107E-3</v>
+      </c>
+      <c r="H24" s="29">
+        <f t="shared" si="3"/>
+        <v>2.587336082044565E-2</v>
+      </c>
+      <c r="I24" s="29">
+        <f t="shared" si="3"/>
+        <v>6.4285745736666214E-3</v>
+      </c>
+      <c r="J24" s="29">
+        <f t="shared" si="3"/>
+        <v>6.9504361997890909E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="B25" s="29">
+        <f t="shared" si="3"/>
+        <v>5.6486953724922608E-2</v>
+      </c>
+      <c r="C25" s="29">
+        <f t="shared" si="3"/>
+        <v>9.3801379969365259E-2</v>
+      </c>
+      <c r="D25" s="29">
+        <f t="shared" si="3"/>
+        <v>4.0994728876363448E-2</v>
+      </c>
+      <c r="E25" s="29">
+        <f t="shared" si="3"/>
+        <v>0.10160172125268944</v>
+      </c>
+      <c r="F25" s="29">
+        <f t="shared" si="3"/>
+        <v>0.13225224955121406</v>
+      </c>
+      <c r="G25" s="29">
+        <f t="shared" si="3"/>
+        <v>3.3318744617469753E-2</v>
+      </c>
+      <c r="H25" s="29">
+        <f t="shared" si="3"/>
+        <v>5.4831579417412145E-2</v>
+      </c>
+      <c r="I25" s="29">
+        <f t="shared" si="3"/>
+        <v>0.20840029765180904</v>
+      </c>
+      <c r="J25" s="29">
+        <f t="shared" si="3"/>
+        <v>0.14188476656121179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>1</v>
+      </c>
+      <c r="B26" s="29">
+        <f t="shared" si="3"/>
+        <v>7.047802838419169E-2</v>
+      </c>
+      <c r="C26" s="29">
+        <f t="shared" si="3"/>
+        <v>6.7171624906901262E-2</v>
+      </c>
+      <c r="D26" s="29">
+        <f t="shared" si="3"/>
+        <v>5.936537758989615E-2</v>
+      </c>
+      <c r="E26" s="29">
+        <f t="shared" si="3"/>
+        <v>0.14009084389194357</v>
+      </c>
+      <c r="F26" s="29">
+        <f t="shared" si="3"/>
+        <v>0.14862590928340411</v>
+      </c>
+      <c r="G26" s="29">
+        <f t="shared" si="3"/>
+        <v>3.0509240304386495E-2</v>
+      </c>
+      <c r="H26" s="29">
+        <f t="shared" si="3"/>
+        <v>9.8722891207597155E-2</v>
+      </c>
+      <c r="I26" s="29">
+        <f t="shared" si="3"/>
+        <v>0.18184940403591196</v>
+      </c>
+      <c r="J26" s="29">
+        <f t="shared" si="3"/>
+        <v>0.1102962323842393</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="B27" s="29">
+        <f t="shared" si="3"/>
+        <v>8.5132472962650252E-2</v>
+      </c>
+      <c r="C27" s="29">
+        <f t="shared" si="3"/>
+        <v>5.6379196469976536E-2</v>
+      </c>
+      <c r="D27" s="29">
+        <f t="shared" si="3"/>
+        <v>0.1082928865925578</v>
+      </c>
+      <c r="E27" s="29">
+        <f t="shared" si="3"/>
+        <v>0.19191768268387918</v>
+      </c>
+      <c r="F27" s="29">
+        <f t="shared" si="3"/>
+        <v>0.16183277055514539</v>
+      </c>
+      <c r="G27" s="29">
+        <f t="shared" si="3"/>
+        <v>0.10023859609493019</v>
+      </c>
+      <c r="H27" s="29">
+        <f t="shared" si="3"/>
+        <v>0.16070843814655492</v>
+      </c>
+      <c r="I27" s="29">
+        <f t="shared" si="3"/>
+        <v>0.16974519067768626</v>
+      </c>
+      <c r="J27" s="29">
+        <f t="shared" si="3"/>
+        <v>0.11927587639408176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="B28" s="29">
+        <f t="shared" si="3"/>
+        <v>0.10734531419611626</v>
+      </c>
+      <c r="C28" s="29">
+        <f t="shared" si="3"/>
+        <v>4.2298449993676317E-2</v>
+      </c>
+      <c r="D28" s="29">
+        <f t="shared" si="3"/>
+        <v>0.16781483221126248</v>
+      </c>
+      <c r="E28" s="29">
+        <f t="shared" si="3"/>
+        <v>0.18674794804366879</v>
+      </c>
+      <c r="F28" s="29">
+        <f t="shared" si="3"/>
+        <v>0.14825863561580177</v>
+      </c>
+      <c r="G28" s="29">
+        <f t="shared" si="3"/>
+        <v>0.10299162795950927</v>
+      </c>
+      <c r="H28" s="29">
+        <f t="shared" si="3"/>
+        <v>0.20782787312266496</v>
+      </c>
+      <c r="I28" s="29">
+        <f t="shared" si="3"/>
+        <v>9.2465798662328129E-4</v>
+      </c>
+      <c r="J28" s="29">
+        <f t="shared" si="3"/>
+        <v>0.11526539481673219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.27851485546576604</v>
+      </c>
+      <c r="C29" s="30">
+        <f t="shared" si="3"/>
+        <v>6.4199491294388789E-2</v>
+      </c>
+      <c r="D29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.60330880434215328</v>
+      </c>
+      <c r="E29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.22113315802055941</v>
+      </c>
+      <c r="F29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.1845362795177472</v>
+      </c>
+      <c r="G29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.7198190058025441</v>
+      </c>
+      <c r="H29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.41098566601670061</v>
+      </c>
+      <c r="I29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.10069965787654496</v>
+      </c>
+      <c r="J29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.18264468091905539</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="P32" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="N33" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P33" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q33" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="R33" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="18">
+        <f>SUM(B19:B23)</f>
+        <v>0.402042375266353</v>
+      </c>
+      <c r="C34" s="18">
+        <f t="shared" ref="C34:J34" si="4">SUM(C19:C23)</f>
+        <v>0.5811540028948442</v>
+      </c>
+      <c r="D34" s="18">
+        <f t="shared" si="4"/>
+        <v>3.5227806481916393E-3</v>
+      </c>
+      <c r="E34" s="18">
+        <f t="shared" si="4"/>
+        <v>8.9947406167822125E-2</v>
+      </c>
+      <c r="F34" s="18">
+        <f t="shared" si="4"/>
+        <v>0.13483440829588766</v>
+      </c>
+      <c r="G34" s="18">
+        <f t="shared" si="4"/>
+        <v>7.1084694554644154E-3</v>
+      </c>
+      <c r="H34" s="18">
+        <f t="shared" si="4"/>
+        <v>4.1050191268624497E-2</v>
+      </c>
+      <c r="I34" s="18">
+        <f t="shared" si="4"/>
+        <v>0.33195221719775792</v>
+      </c>
+      <c r="J34" s="18">
+        <f t="shared" si="4"/>
+        <v>0.26112868692678876</v>
+      </c>
+      <c r="L34" s="18">
+        <f>AVERAGE(B34:J34)</f>
+        <v>0.20586005979130381</v>
+      </c>
+      <c r="M34" s="18">
+        <f>MIN(B34:J34)</f>
+        <v>3.5227806481916393E-3</v>
+      </c>
+      <c r="N34" s="18">
+        <f>MAX(B34:J34)</f>
+        <v>0.5811540028948442</v>
+      </c>
+      <c r="P34" s="33">
+        <f>L34*100</f>
+        <v>20.58600597913038</v>
+      </c>
+      <c r="Q34" s="33">
+        <f>M34*100</f>
+        <v>0.35227806481916396</v>
+      </c>
+      <c r="R34" s="33">
+        <f>N34*100</f>
+        <v>58.11540028948442</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="18">
+        <f>SUM(B24:B28)</f>
+        <v>0.31944276926788084</v>
+      </c>
+      <c r="C35" s="18">
+        <f t="shared" ref="C35:J35" si="5">SUM(C24:C28)</f>
+        <v>0.35464650581076718</v>
+      </c>
+      <c r="D35" s="18">
+        <f t="shared" si="5"/>
+        <v>0.39316841500965505</v>
+      </c>
+      <c r="E35" s="18">
+        <f t="shared" si="5"/>
+        <v>0.68891943581161841</v>
+      </c>
+      <c r="F35" s="18">
+        <f t="shared" si="5"/>
+        <v>0.68062931218636513</v>
+      </c>
+      <c r="G35" s="18">
+        <f t="shared" si="5"/>
+        <v>0.27307252474199151</v>
+      </c>
+      <c r="H35" s="18">
+        <f t="shared" si="5"/>
+        <v>0.54796414271467475</v>
+      </c>
+      <c r="I35" s="18">
+        <f t="shared" si="5"/>
+        <v>0.56734812492569719</v>
+      </c>
+      <c r="J35" s="18">
+        <f t="shared" si="5"/>
+        <v>0.55622663215415591</v>
+      </c>
+      <c r="L35" s="18">
+        <f t="shared" ref="L35:L36" si="6">AVERAGE(B35:J35)</f>
+        <v>0.48682420695808953</v>
+      </c>
+      <c r="M35" s="18">
+        <f t="shared" ref="M35:M36" si="7">MIN(B35:J35)</f>
+        <v>0.27307252474199151</v>
+      </c>
+      <c r="N35" s="18">
+        <f t="shared" ref="N35:N36" si="8">MAX(B35:J35)</f>
+        <v>0.68891943581161841</v>
+      </c>
+      <c r="P35" s="33">
+        <f t="shared" ref="P35:P36" si="9">L35*100</f>
+        <v>48.68242069580895</v>
+      </c>
+      <c r="Q35" s="33">
+        <f t="shared" ref="Q35:Q36" si="10">M35*100</f>
+        <v>27.307252474199149</v>
+      </c>
+      <c r="R35" s="33">
+        <f t="shared" ref="R35:R36" si="11">N35*100</f>
+        <v>68.89194358116184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="18">
+        <f>B29</f>
+        <v>0.27851485546576604</v>
+      </c>
+      <c r="C36" s="18">
+        <f t="shared" ref="C36:J36" si="12">C29</f>
+        <v>6.4199491294388789E-2</v>
+      </c>
+      <c r="D36" s="18">
+        <f t="shared" si="12"/>
+        <v>0.60330880434215328</v>
+      </c>
+      <c r="E36" s="18">
+        <f t="shared" si="12"/>
+        <v>0.22113315802055941</v>
+      </c>
+      <c r="F36" s="18">
+        <f t="shared" si="12"/>
+        <v>0.1845362795177472</v>
+      </c>
+      <c r="G36" s="18">
+        <f t="shared" si="12"/>
+        <v>0.7198190058025441</v>
+      </c>
+      <c r="H36" s="18">
+        <f t="shared" si="12"/>
+        <v>0.41098566601670061</v>
+      </c>
+      <c r="I36" s="18">
+        <f t="shared" si="12"/>
+        <v>0.10069965787654496</v>
+      </c>
+      <c r="J36" s="18">
+        <f t="shared" si="12"/>
+        <v>0.18264468091905539</v>
+      </c>
+      <c r="L36" s="18">
+        <f t="shared" si="6"/>
+        <v>0.30731573325060663</v>
+      </c>
+      <c r="M36" s="18">
+        <f t="shared" si="7"/>
+        <v>6.4199491294388789E-2</v>
+      </c>
+      <c r="N36" s="18">
+        <f t="shared" si="8"/>
+        <v>0.7198190058025441</v>
+      </c>
+      <c r="P36" s="33">
+        <f t="shared" si="9"/>
+        <v>30.731573325060662</v>
+      </c>
+      <c r="Q36" s="33">
+        <f t="shared" si="10"/>
+        <v>6.4199491294388791</v>
+      </c>
+      <c r="R36" s="33">
+        <f t="shared" si="11"/>
+        <v>71.981900580254404</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="18">
+        <f>SUM(B34:B36)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C37" s="18">
+        <f t="shared" ref="C37:J37" si="13">SUM(C34:C36)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D37" s="18">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="F37" s="18">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G37" s="18">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="H37" s="18">
+        <f t="shared" si="13"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I37" s="18">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="J37" s="18">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <f>SUM(P34:P36)</f>
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A32:J32"/>
+    <mergeCell ref="P32:R32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1069,16 +2045,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1092,7 +2068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>11.2</v>
       </c>
@@ -1104,7 +2080,7 @@
         <v>24.492999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -1116,7 +2092,7 @@
         <v>10.259</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5.6</v>
       </c>
@@ -1128,7 +2104,7 @@
         <v>17.543800000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1140,7 +2116,7 @@
         <v>16.167000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2.8</v>
       </c>
@@ -1152,7 +2128,7 @@
         <v>14.247999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -1164,7 +2140,7 @@
         <v>13.518000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -1173,7 +2149,7 @@
         <v>0.56200000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1182,7 +2158,7 @@
         <v>0.70120000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.71</v>
       </c>
@@ -1190,7 +2166,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.5</v>
       </c>
@@ -1199,7 +2175,7 @@
         <v>1.0680000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.25</v>
       </c>
@@ -1210,7 +2186,7 @@
         <v>9.1370000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +2198,7 @@
         <v>1.9748000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1238,7 +2214,7 @@
         <v>107.34060000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1252,12 +2228,12 @@
         <v>120.92940000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1268,7 +2244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>11.2</v>
       </c>
@@ -1282,7 +2258,7 @@
         <v>0.22818020394892516</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>8</v>
       </c>
@@ -1296,7 +2272,7 @@
         <v>9.5574274785123245E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>5.6</v>
       </c>
@@ -1310,7 +2286,7 @@
         <v>0.1634404875694751</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>4</v>
       </c>
@@ -1324,7 +2300,7 @@
         <v>0.1506140267522261</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>2.8</v>
       </c>
@@ -1338,7 +2314,7 @@
         <v>0.13273635511633061</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>2</v>
       </c>
@@ -1352,13 +2328,13 @@
         <v>0.1259355733059066</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>1.4</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="4">
-        <f t="shared" si="0"/>
+        <f>C9/$C$15</f>
         <v>5.0543204547089722E-2</v>
       </c>
       <c r="D26" s="6">
@@ -1366,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>1</v>
       </c>
@@ -1380,7 +2356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>0.71</v>
       </c>
@@ -1394,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>0.5</v>
       </c>
@@ -1408,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>0.25</v>
       </c>
@@ -1422,7 +2398,7 @@
         <v>8.5121566303896196E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -1436,7 +2412,7 @@
         <v>1.8397512218116911E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -1449,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>7</v>
       </c>
@@ -1466,7 +2442,7 @@
         <v>0.62810951606671472</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>8</v>
       </c>
@@ -1483,7 +2459,7 @@
         <v>0.31008002914086819</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>9</v>
       </c>
@@ -1500,7 +2476,7 @@
         <v>6.1810454792416966E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C37" s="1">
         <f>SUM(C34:C36)</f>
         <v>1</v>
@@ -1510,12 +2486,12 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -1526,7 +2502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>11.2</v>
       </c>
@@ -1536,7 +2512,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>8</v>
       </c>
@@ -1546,7 +2522,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>5.6</v>
       </c>
@@ -1556,7 +2532,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>4</v>
       </c>
@@ -1566,7 +2542,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>2.8</v>
       </c>
@@ -1576,7 +2552,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>2</v>
       </c>
@@ -1586,7 +2562,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>1.4</v>
       </c>
@@ -1596,7 +2572,7 @@
         <v>0.41028131520253253</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>1</v>
       </c>
@@ -1606,7 +2582,7 @@
         <v>0.47334340600043168</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>0.71</v>
       </c>
@@ -1616,7 +2592,7 @@
         <v>0.54951795093172173</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>0.5</v>
       </c>
@@ -1626,7 +2602,7 @@
         <v>0.64556802647672495</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>0.25</v>
       </c>
@@ -1636,7 +2612,7 @@
         <v>0.89477660263328296</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
@@ -1659,12 +2635,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1678,7 +2654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>11.2</v>
       </c>
@@ -1692,7 +2668,7 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -1704,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5.6</v>
       </c>
@@ -1716,7 +2692,7 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1728,7 +2704,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2.8</v>
       </c>
@@ -1740,7 +2716,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -1752,7 +2728,7 @@
         <v>0.50700000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -1764,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1776,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.71</v>
       </c>
@@ -1787,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.5</v>
       </c>
@@ -1799,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.25</v>
       </c>
@@ -1810,7 +2786,7 @@
         <v>9.1370000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1822,7 +2798,7 @@
         <v>1.9748000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
smoothed and calculated kde for bedload spring
</commit_message>
<xml_diff>
--- a/Bedload/bedloadGSDs.xlsx
+++ b/Bedload/bedloadGSDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Bedload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Bedload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06C5613-8636-4475-9850-132058BFF747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C8A429-A787-465C-93B3-43EE4CFA907C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
   <si>
     <t>pan</t>
   </si>
@@ -139,7 +139,13 @@
     <t>Fines (&lt;0.2mm)</t>
   </si>
   <si>
-    <t>%</t>
+    <t>Percent Retained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL </t>
+  </si>
+  <si>
+    <t>Cumulative Percent Retained</t>
   </si>
 </sst>
 </file>
@@ -366,12 +372,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,12 +393,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,32 +683,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699A0717-E7CB-4E57-A578-ABA98CA0B5D1}">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -735,8 +742,38 @@
       <c r="J2" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>11.2</v>
       </c>
@@ -767,8 +804,47 @@
       <c r="J3" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3" s="11">
+        <v>11.2</v>
+      </c>
+      <c r="M3">
+        <f>B3/(B$14-B13)</f>
+        <v>0.55724276280961793</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:U12" si="0">C3/C$14</f>
+        <v>0.17209567038124818</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>8</v>
       </c>
@@ -799,8 +875,47 @@
       <c r="J4" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L4" s="16">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M12" si="1">B4/B$14</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>7.2083023004173644E-2</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>4.3855207365561338E-2</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>5.6</v>
       </c>
@@ -831,8 +946,47 @@
       <c r="J5" s="17">
         <v>0.29499999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L5" s="16">
+        <v>5.6</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0.12324166327061173</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>3.7990338453927769E-2</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>1.8103538097435361E-2</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>4.561646067341521E-2</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>4.7135142044546705E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -863,8 +1017,47 @@
       <c r="J6" s="17">
         <v>0.56530000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L6" s="16">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0.11361560405278175</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>3.9519396172108937E-2</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>1.1070508908503638E-2</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>6.8997098335175311E-2</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>9.0323714568753405E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>2.8</v>
       </c>
@@ -895,8 +1088,47 @@
       <c r="J7" s="17">
         <v>0.77400000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L7" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.10011804218602889</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>3.5227806481916393E-3</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>8.9947406167822125E-2</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>5.7324673669850959E-2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>7.1084694554644154E-3</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>1.18761442626855E-2</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>0.17348345082360608</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>0.12366983031348865</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>2</v>
       </c>
@@ -927,8 +1159,47 @@
       <c r="J8" s="17">
         <v>0.435</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L8" s="16">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>9.499585447084781E-2</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>1.6700589739575181E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>6.8561239939437399E-2</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>8.9659747180799831E-2</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>6.0143157656958107E-3</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>2.587336082044565E-2</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>6.4285745736666214E-3</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>6.9504361997890909E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>1.4</v>
       </c>
@@ -959,8 +1230,47 @@
       <c r="J9" s="17">
         <v>0.88800000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L9" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>5.6486953724922608E-2</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>9.3801379969365259E-2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>4.0994728876363448E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0.10160172125268944</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0.13225224955121406</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>3.3318744617469753E-2</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>5.4831579417412145E-2</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>0.20840029765180904</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>0.14188476656121179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>1</v>
       </c>
@@ -991,8 +1301,47 @@
       <c r="J10" s="17">
         <v>0.69030000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="16">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>7.047802838419169E-2</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>6.7171624906901262E-2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>5.936537758989615E-2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>0.14009084389194357</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>0.14862590928340411</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>3.0509240304386495E-2</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>9.8722891207597155E-2</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>0.18184940403591196</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>0.1102962323842393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>0.7</v>
       </c>
@@ -1023,8 +1372,47 @@
       <c r="J11" s="17">
         <v>0.74650000000000005</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>8.5132472962650252E-2</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>5.6379196469976536E-2</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>0.1082928865925578</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>0.19191768268387918</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>0.16183277055514539</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>0.10023859609493019</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>0.16070843814655492</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>0.16974519067768626</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="0"/>
+        <v>0.11927587639408176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>0.5</v>
       </c>
@@ -1055,8 +1443,47 @@
       <c r="J12" s="17">
         <v>0.72140000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L12" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>0.10734531419611626</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>4.2298449993676317E-2</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0.16781483221126248</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>0.18674794804366879</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>0.14825863561580177</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>0.10299162795950927</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>0.20782787312266496</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>9.2465798662328129E-4</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>0.11526539481673219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>0</v>
       </c>
@@ -1087,8 +1514,47 @@
       <c r="J13" s="17">
         <v>1.1431</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L13" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="33">
+        <f>SUM(M3:M12)</f>
+        <v>0.87668553207749877</v>
+      </c>
+      <c r="N13" s="33">
+        <f t="shared" ref="N13:U13" si="2">SUM(N3:N12)</f>
+        <v>0.93580050870561127</v>
+      </c>
+      <c r="O13" s="33">
+        <f t="shared" si="2"/>
+        <v>0.39669119565784672</v>
+      </c>
+      <c r="P13" s="33">
+        <f t="shared" si="2"/>
+        <v>0.77886684197944056</v>
+      </c>
+      <c r="Q13" s="33">
+        <f t="shared" si="2"/>
+        <v>0.8154637204822528</v>
+      </c>
+      <c r="R13" s="33">
+        <f t="shared" si="2"/>
+        <v>0.28018099419745596</v>
+      </c>
+      <c r="S13" s="33">
+        <f t="shared" si="2"/>
+        <v>0.58901433398329928</v>
+      </c>
+      <c r="T13" s="33">
+        <f t="shared" si="2"/>
+        <v>0.89930034212345511</v>
+      </c>
+      <c r="U13" s="33">
+        <f t="shared" si="2"/>
+        <v>0.81735531908094461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
@@ -1097,81 +1563,84 @@
         <v>9.9492000000000012</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" ref="C14:J14" si="0">SUM(C3:C13)</f>
+        <f t="shared" ref="C14:J14" si="3">SUM(C3:C13)</f>
         <v>142.32199999999997</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.6643999999999997</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10.039200000000001</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>26.6831</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14.1662</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>53.746400000000001</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>22.711099999999998</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.2585999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="21">
-        <f>SUM(B3:B13)/1000</f>
+        <f t="shared" ref="B15:J15" si="4">SUM(B3:B13)/1000</f>
         <v>9.9492000000000018E-3</v>
       </c>
       <c r="C15" s="22">
-        <f>SUM(C3:C13)/1000</f>
+        <f t="shared" si="4"/>
         <v>0.14232199999999998</v>
       </c>
       <c r="D15" s="22">
-        <f>SUM(D3:D13)/1000</f>
+        <f t="shared" si="4"/>
         <v>7.6644E-3</v>
       </c>
       <c r="E15" s="22">
-        <f>SUM(E3:E13)/1000</f>
+        <f t="shared" si="4"/>
         <v>1.0039200000000002E-2</v>
       </c>
       <c r="F15" s="22">
-        <f>SUM(F3:F13)/1000</f>
+        <f t="shared" si="4"/>
         <v>2.6683100000000001E-2</v>
       </c>
       <c r="G15" s="22">
-        <f>SUM(G3:G13)/1000</f>
+        <f t="shared" si="4"/>
         <v>1.41662E-2</v>
       </c>
       <c r="H15" s="22">
-        <f>SUM(H3:H13)/1000</f>
+        <f t="shared" si="4"/>
         <v>5.37464E-2</v>
       </c>
       <c r="I15" s="22">
-        <f>SUM(I3:I13)/1000</f>
+        <f t="shared" si="4"/>
         <v>2.2711099999999998E-2</v>
       </c>
       <c r="J15" s="22">
-        <f>SUM(J3:J13)/1000</f>
+        <f t="shared" si="4"/>
         <v>6.2585999999999996E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
+      <c r="L15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -1181,23 +1650,91 @@
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="L16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U16" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="L17" s="11">
+        <v>11.2</v>
+      </c>
+      <c r="M17">
+        <f>M3</f>
+        <v>0.55724276280961793</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ref="N17:U17" si="5">N3</f>
+        <v>0.17209567038124818</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
@@ -1228,569 +1765,897 @@
       <c r="J18" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L18" s="16">
+        <v>8</v>
+      </c>
+      <c r="M18">
+        <f>M4+M17</f>
+        <v>0.55724276280961793</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:U26" si="6">N4+N17</f>
+        <v>0.24417869338542181</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="6"/>
+        <v>4.3855207365561338E-2</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>11.2</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="26">
         <f>B3/B$14</f>
         <v>0.402042375266353</v>
       </c>
-      <c r="C19" s="28">
-        <f t="shared" ref="C19:J19" si="1">C3/C$14</f>
+      <c r="C19" s="26">
+        <f t="shared" ref="C19:J19" si="7">C3/C$14</f>
         <v>0.17209567038124818</v>
       </c>
-      <c r="D19" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D19" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="16">
+        <v>5.6</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ref="M19:M26" si="8">M5+M18</f>
+        <v>0.55724276280961793</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="6"/>
+        <v>0.36742035665603356</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="6"/>
+        <v>3.7990338453927769E-2</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="6"/>
+        <v>1.8103538097435361E-2</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="6"/>
+        <v>8.9471668038976548E-2</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="6"/>
+        <v>4.7135142044546705E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>8</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="26">
         <f>B4/B$14</f>
         <v>0</v>
       </c>
-      <c r="C20" s="28">
-        <f t="shared" ref="C20:J20" si="2">C4/C$14</f>
+      <c r="C20" s="26">
+        <f t="shared" ref="C20:J20" si="9">C4/C$14</f>
         <v>7.2083023004173644E-2</v>
       </c>
-      <c r="D20" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="28">
-        <f t="shared" si="2"/>
+      <c r="D20" s="26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="26">
+        <f t="shared" si="9"/>
         <v>4.3855207365561338E-2</v>
       </c>
-      <c r="J20" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J20" s="26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="16">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="8"/>
+        <v>0.55724276280961793</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="6"/>
+        <v>0.48103596070881532</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="6"/>
+        <v>7.7509734626036705E-2</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="6"/>
+        <v>2.9174047005939001E-2</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="6"/>
+        <v>0.15846876637415186</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="6"/>
+        <v>0.1374588566133001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>5.6</v>
       </c>
-      <c r="B21" s="28">
-        <f t="shared" ref="B20:J30" si="3">B5/B$14</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="28">
-        <f t="shared" si="3"/>
+      <c r="B21" s="26">
+        <f t="shared" ref="B21:J30" si="10">B5/B$14</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="26">
+        <f t="shared" si="10"/>
         <v>0.12324166327061173</v>
       </c>
-      <c r="D21" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="28">
-        <f t="shared" si="3"/>
+      <c r="D21" s="26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="26">
+        <f t="shared" si="10"/>
         <v>3.7990338453927769E-2</v>
       </c>
-      <c r="G21" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="28">
-        <f t="shared" si="3"/>
+      <c r="G21" s="26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="26">
+        <f t="shared" si="10"/>
         <v>1.8103538097435361E-2</v>
       </c>
-      <c r="I21" s="28">
-        <f t="shared" si="3"/>
+      <c r="I21" s="26">
+        <f t="shared" si="10"/>
         <v>4.561646067341521E-2</v>
       </c>
-      <c r="J21" s="28">
-        <f t="shared" si="3"/>
+      <c r="J21" s="26">
+        <f t="shared" si="10"/>
         <v>4.7135142044546705E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L21" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="8"/>
+        <v>0.55724276280961793</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="6"/>
+        <v>0.5811540028948442</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="6"/>
+        <v>3.5227806481916393E-3</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="6"/>
+        <v>8.9947406167822125E-2</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="6"/>
+        <v>0.13483440829588766</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="6"/>
+        <v>7.1084694554644154E-3</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="6"/>
+        <v>4.1050191268624497E-2</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="6"/>
+        <v>0.33195221719775792</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="6"/>
+        <v>0.26112868692678876</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>4</v>
       </c>
-      <c r="B22" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C22" s="28">
-        <f t="shared" si="3"/>
+      <c r="B22" s="26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C22" s="26">
+        <f t="shared" si="10"/>
         <v>0.11361560405278175</v>
       </c>
-      <c r="D22" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="28">
-        <f t="shared" si="3"/>
+      <c r="D22" s="26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="26">
+        <f t="shared" si="10"/>
         <v>3.9519396172108937E-2</v>
       </c>
-      <c r="G22" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="28">
-        <f t="shared" si="3"/>
+      <c r="G22" s="26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="26">
+        <f t="shared" si="10"/>
         <v>1.1070508908503638E-2</v>
       </c>
-      <c r="I22" s="28">
-        <f t="shared" si="3"/>
+      <c r="I22" s="26">
+        <f t="shared" si="10"/>
         <v>6.8997098335175311E-2</v>
       </c>
-      <c r="J22" s="28">
-        <f t="shared" si="3"/>
+      <c r="J22" s="26">
+        <f t="shared" si="10"/>
         <v>9.0323714568753405E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L22" s="16">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="8"/>
+        <v>0.55724276280961793</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="6"/>
+        <v>0.676149857365692</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="6"/>
+        <v>2.022337038776682E-2</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="6"/>
+        <v>0.15850864610725951</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="6"/>
+        <v>0.2244941554766875</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="6"/>
+        <v>1.3122785221160227E-2</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="6"/>
+        <v>6.6923552089070151E-2</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="6"/>
+        <v>0.33838079177142455</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="6"/>
+        <v>0.33063304892467965</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>2.8</v>
       </c>
-      <c r="B23" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C23" s="28">
-        <f t="shared" si="3"/>
+      <c r="B23" s="26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C23" s="26">
+        <f t="shared" si="10"/>
         <v>0.10011804218602889</v>
       </c>
-      <c r="D23" s="28">
-        <f t="shared" si="3"/>
+      <c r="D23" s="26">
+        <f t="shared" si="10"/>
         <v>3.5227806481916393E-3</v>
       </c>
-      <c r="E23" s="28">
-        <f t="shared" si="3"/>
+      <c r="E23" s="26">
+        <f t="shared" si="10"/>
         <v>8.9947406167822125E-2</v>
       </c>
-      <c r="F23" s="28">
-        <f t="shared" si="3"/>
+      <c r="F23" s="26">
+        <f t="shared" si="10"/>
         <v>5.7324673669850959E-2</v>
       </c>
-      <c r="G23" s="28">
-        <f t="shared" si="3"/>
+      <c r="G23" s="26">
+        <f t="shared" si="10"/>
         <v>7.1084694554644154E-3</v>
       </c>
-      <c r="H23" s="28">
-        <f t="shared" si="3"/>
+      <c r="H23" s="26">
+        <f t="shared" si="10"/>
         <v>1.18761442626855E-2</v>
       </c>
-      <c r="I23" s="28">
-        <f t="shared" si="3"/>
+      <c r="I23" s="26">
+        <f t="shared" si="10"/>
         <v>0.17348345082360608</v>
       </c>
-      <c r="J23" s="28">
-        <f t="shared" si="3"/>
+      <c r="J23" s="26">
+        <f t="shared" si="10"/>
         <v>0.12366983031348865</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L23" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="8"/>
+        <v>0.61372971653454056</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="6"/>
+        <v>0.76995123733505721</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="6"/>
+        <v>6.1218099264130271E-2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="6"/>
+        <v>0.26011036735994897</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="6"/>
+        <v>0.35674640502790156</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="6"/>
+        <v>4.644152983862998E-2</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="6"/>
+        <v>0.12175513150648229</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="6"/>
+        <v>0.54678108942323356</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="6"/>
+        <v>0.47251781548589145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>2</v>
       </c>
-      <c r="B24" s="29">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="C24" s="29">
-        <f t="shared" si="3"/>
+      <c r="B24" s="27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C24" s="27">
+        <f t="shared" si="10"/>
         <v>9.499585447084781E-2</v>
       </c>
-      <c r="D24" s="29">
-        <f t="shared" si="3"/>
+      <c r="D24" s="27">
+        <f t="shared" si="10"/>
         <v>1.6700589739575181E-2</v>
       </c>
-      <c r="E24" s="29">
-        <f t="shared" si="3"/>
+      <c r="E24" s="27">
+        <f t="shared" si="10"/>
         <v>6.8561239939437399E-2</v>
       </c>
-      <c r="F24" s="29">
-        <f t="shared" si="3"/>
+      <c r="F24" s="27">
+        <f t="shared" si="10"/>
         <v>8.9659747180799831E-2</v>
       </c>
-      <c r="G24" s="29">
-        <f t="shared" si="3"/>
+      <c r="G24" s="27">
+        <f t="shared" si="10"/>
         <v>6.0143157656958107E-3</v>
       </c>
-      <c r="H24" s="29">
-        <f t="shared" si="3"/>
+      <c r="H24" s="27">
+        <f t="shared" si="10"/>
         <v>2.587336082044565E-2</v>
       </c>
-      <c r="I24" s="29">
-        <f t="shared" si="3"/>
+      <c r="I24" s="27">
+        <f t="shared" si="10"/>
         <v>6.4285745736666214E-3</v>
       </c>
-      <c r="J24" s="29">
-        <f t="shared" si="3"/>
+      <c r="J24" s="27">
+        <f t="shared" si="10"/>
         <v>6.9504361997890909E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L24" s="16">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="8"/>
+        <v>0.68420774491873226</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="6"/>
+        <v>0.83712286224195842</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="6"/>
+        <v>0.12058347685402643</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="6"/>
+        <v>0.40020121125189256</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="6"/>
+        <v>0.50537231431130569</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="6"/>
+        <v>7.6950770143016475E-2</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="6"/>
+        <v>0.22047802271407946</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="6"/>
+        <v>0.72863049345914555</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="6"/>
+        <v>0.58281404787013069</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>1.4</v>
       </c>
-      <c r="B25" s="29">
-        <f t="shared" si="3"/>
+      <c r="B25" s="27">
+        <f t="shared" si="10"/>
         <v>5.6486953724922608E-2</v>
       </c>
-      <c r="C25" s="29">
-        <f t="shared" si="3"/>
+      <c r="C25" s="27">
+        <f t="shared" si="10"/>
         <v>9.3801379969365259E-2</v>
       </c>
-      <c r="D25" s="29">
-        <f t="shared" si="3"/>
+      <c r="D25" s="27">
+        <f t="shared" si="10"/>
         <v>4.0994728876363448E-2</v>
       </c>
-      <c r="E25" s="29">
-        <f t="shared" si="3"/>
+      <c r="E25" s="27">
+        <f t="shared" si="10"/>
         <v>0.10160172125268944</v>
       </c>
-      <c r="F25" s="29">
-        <f t="shared" si="3"/>
+      <c r="F25" s="27">
+        <f t="shared" si="10"/>
         <v>0.13225224955121406</v>
       </c>
-      <c r="G25" s="29">
-        <f t="shared" si="3"/>
+      <c r="G25" s="27">
+        <f t="shared" si="10"/>
         <v>3.3318744617469753E-2</v>
       </c>
-      <c r="H25" s="29">
-        <f t="shared" si="3"/>
+      <c r="H25" s="27">
+        <f t="shared" si="10"/>
         <v>5.4831579417412145E-2</v>
       </c>
-      <c r="I25" s="29">
-        <f t="shared" si="3"/>
+      <c r="I25" s="27">
+        <f t="shared" si="10"/>
         <v>0.20840029765180904</v>
       </c>
-      <c r="J25" s="29">
-        <f t="shared" si="3"/>
+      <c r="J25" s="27">
+        <f t="shared" si="10"/>
         <v>0.14188476656121179</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L25" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="8"/>
+        <v>0.76934021788138252</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="6"/>
+        <v>0.893502058711935</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="6"/>
+        <v>0.22887636344658424</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="6"/>
+        <v>0.59211889393577177</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="6"/>
+        <v>0.66720508486645103</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="6"/>
+        <v>0.17718936623794668</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="6"/>
+        <v>0.38118646086063435</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="6"/>
+        <v>0.89837568413683178</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="6"/>
+        <v>0.70208992426421246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>1</v>
       </c>
-      <c r="B26" s="29">
-        <f t="shared" si="3"/>
+      <c r="B26" s="27">
+        <f t="shared" si="10"/>
         <v>7.047802838419169E-2</v>
       </c>
-      <c r="C26" s="29">
-        <f t="shared" si="3"/>
+      <c r="C26" s="27">
+        <f t="shared" si="10"/>
         <v>6.7171624906901262E-2</v>
       </c>
-      <c r="D26" s="29">
-        <f t="shared" si="3"/>
+      <c r="D26" s="27">
+        <f t="shared" si="10"/>
         <v>5.936537758989615E-2</v>
       </c>
-      <c r="E26" s="29">
-        <f t="shared" si="3"/>
+      <c r="E26" s="27">
+        <f t="shared" si="10"/>
         <v>0.14009084389194357</v>
       </c>
-      <c r="F26" s="29">
-        <f t="shared" si="3"/>
+      <c r="F26" s="27">
+        <f t="shared" si="10"/>
         <v>0.14862590928340411</v>
       </c>
-      <c r="G26" s="29">
-        <f t="shared" si="3"/>
+      <c r="G26" s="27">
+        <f t="shared" si="10"/>
         <v>3.0509240304386495E-2</v>
       </c>
-      <c r="H26" s="29">
-        <f t="shared" si="3"/>
+      <c r="H26" s="27">
+        <f t="shared" si="10"/>
         <v>9.8722891207597155E-2</v>
       </c>
-      <c r="I26" s="29">
-        <f t="shared" si="3"/>
+      <c r="I26" s="27">
+        <f t="shared" si="10"/>
         <v>0.18184940403591196</v>
       </c>
-      <c r="J26" s="29">
-        <f t="shared" si="3"/>
+      <c r="J26" s="27">
+        <f t="shared" si="10"/>
         <v>0.1102962323842393</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L26" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="8"/>
+        <v>0.87668553207749877</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="6"/>
+        <v>0.93580050870561127</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="6"/>
+        <v>0.39669119565784672</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="6"/>
+        <v>0.77886684197944056</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="6"/>
+        <v>0.8154637204822528</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="6"/>
+        <v>0.28018099419745596</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="6"/>
+        <v>0.58901433398329928</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="6"/>
+        <v>0.89930034212345511</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="6"/>
+        <v>0.81735531908094461</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>0.7</v>
       </c>
-      <c r="B27" s="29">
-        <f t="shared" si="3"/>
+      <c r="B27" s="27">
+        <f t="shared" si="10"/>
         <v>8.5132472962650252E-2</v>
       </c>
-      <c r="C27" s="29">
-        <f t="shared" si="3"/>
+      <c r="C27" s="27">
+        <f t="shared" si="10"/>
         <v>5.6379196469976536E-2</v>
       </c>
-      <c r="D27" s="29">
-        <f t="shared" si="3"/>
+      <c r="D27" s="27">
+        <f t="shared" si="10"/>
         <v>0.1082928865925578</v>
       </c>
-      <c r="E27" s="29">
-        <f t="shared" si="3"/>
+      <c r="E27" s="27">
+        <f t="shared" si="10"/>
         <v>0.19191768268387918</v>
       </c>
-      <c r="F27" s="29">
-        <f t="shared" si="3"/>
+      <c r="F27" s="27">
+        <f t="shared" si="10"/>
         <v>0.16183277055514539</v>
       </c>
-      <c r="G27" s="29">
-        <f t="shared" si="3"/>
+      <c r="G27" s="27">
+        <f t="shared" si="10"/>
         <v>0.10023859609493019</v>
       </c>
-      <c r="H27" s="29">
-        <f t="shared" si="3"/>
+      <c r="H27" s="27">
+        <f t="shared" si="10"/>
         <v>0.16070843814655492</v>
       </c>
-      <c r="I27" s="29">
-        <f t="shared" si="3"/>
+      <c r="I27" s="27">
+        <f t="shared" si="10"/>
         <v>0.16974519067768626</v>
       </c>
-      <c r="J27" s="29">
-        <f t="shared" si="3"/>
+      <c r="J27" s="27">
+        <f t="shared" si="10"/>
         <v>0.11927587639408176</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>0.5</v>
       </c>
-      <c r="B28" s="29">
-        <f t="shared" si="3"/>
+      <c r="B28" s="27">
+        <f t="shared" si="10"/>
         <v>0.10734531419611626</v>
       </c>
-      <c r="C28" s="29">
-        <f t="shared" si="3"/>
+      <c r="C28" s="27">
+        <f t="shared" si="10"/>
         <v>4.2298449993676317E-2</v>
       </c>
-      <c r="D28" s="29">
-        <f t="shared" si="3"/>
+      <c r="D28" s="27">
+        <f t="shared" si="10"/>
         <v>0.16781483221126248</v>
       </c>
-      <c r="E28" s="29">
-        <f t="shared" si="3"/>
+      <c r="E28" s="27">
+        <f t="shared" si="10"/>
         <v>0.18674794804366879</v>
       </c>
-      <c r="F28" s="29">
-        <f t="shared" si="3"/>
+      <c r="F28" s="27">
+        <f t="shared" si="10"/>
         <v>0.14825863561580177</v>
       </c>
-      <c r="G28" s="29">
-        <f t="shared" si="3"/>
+      <c r="G28" s="27">
+        <f t="shared" si="10"/>
         <v>0.10299162795950927</v>
       </c>
-      <c r="H28" s="29">
-        <f t="shared" si="3"/>
+      <c r="H28" s="27">
+        <f t="shared" si="10"/>
         <v>0.20782787312266496</v>
       </c>
-      <c r="I28" s="29">
-        <f t="shared" si="3"/>
+      <c r="I28" s="27">
+        <f t="shared" si="10"/>
         <v>9.2465798662328129E-4</v>
       </c>
-      <c r="J28" s="29">
-        <f t="shared" si="3"/>
+      <c r="J28" s="27">
+        <f t="shared" si="10"/>
         <v>0.11526539481673219</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="30">
-        <f t="shared" si="3"/>
+      <c r="B29" s="28">
+        <f t="shared" si="10"/>
         <v>0.27851485546576604</v>
       </c>
-      <c r="C29" s="30">
-        <f t="shared" si="3"/>
+      <c r="C29" s="28">
+        <f t="shared" si="10"/>
         <v>6.4199491294388789E-2</v>
       </c>
-      <c r="D29" s="30">
-        <f t="shared" si="3"/>
+      <c r="D29" s="28">
+        <f t="shared" si="10"/>
         <v>0.60330880434215328</v>
       </c>
-      <c r="E29" s="30">
-        <f t="shared" si="3"/>
+      <c r="E29" s="28">
+        <f t="shared" si="10"/>
         <v>0.22113315802055941</v>
       </c>
-      <c r="F29" s="30">
-        <f t="shared" si="3"/>
+      <c r="F29" s="28">
+        <f t="shared" si="10"/>
         <v>0.1845362795177472</v>
       </c>
-      <c r="G29" s="30">
-        <f t="shared" si="3"/>
+      <c r="G29" s="28">
+        <f t="shared" si="10"/>
         <v>0.7198190058025441</v>
       </c>
-      <c r="H29" s="30">
-        <f t="shared" si="3"/>
+      <c r="H29" s="28">
+        <f t="shared" si="10"/>
         <v>0.41098566601670061</v>
       </c>
-      <c r="I29" s="30">
-        <f t="shared" si="3"/>
+      <c r="I29" s="28">
+        <f t="shared" si="10"/>
         <v>0.10069965787654496</v>
       </c>
-      <c r="J29" s="30">
-        <f t="shared" si="3"/>
+      <c r="J29" s="28">
+        <f t="shared" si="10"/>
         <v>0.18264468091905539</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="23" t="s">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="P32" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q32" s="32"/>
-      <c r="R32" s="32"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="26" t="s">
+      <c r="G33" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="26" t="s">
+      <c r="H33" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="26" t="s">
+      <c r="I33" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="J33" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="L33" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M33" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="N33" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="P33" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q33" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="R33" s="31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>31</v>
       </c>
@@ -1799,63 +2664,39 @@
         <v>0.402042375266353</v>
       </c>
       <c r="C34" s="18">
-        <f t="shared" ref="C34:J34" si="4">SUM(C19:C23)</f>
+        <f t="shared" ref="C34:J34" si="11">SUM(C19:C23)</f>
         <v>0.5811540028948442</v>
       </c>
       <c r="D34" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>3.5227806481916393E-3</v>
       </c>
       <c r="E34" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>8.9947406167822125E-2</v>
       </c>
       <c r="F34" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.13483440829588766</v>
       </c>
       <c r="G34" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>7.1084694554644154E-3</v>
       </c>
       <c r="H34" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>4.1050191268624497E-2</v>
       </c>
       <c r="I34" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.33195221719775792</v>
       </c>
       <c r="J34" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.26112868692678876</v>
       </c>
-      <c r="L34" s="18">
-        <f>AVERAGE(B34:J34)</f>
-        <v>0.20586005979130381</v>
-      </c>
-      <c r="M34" s="18">
-        <f>MIN(B34:J34)</f>
-        <v>3.5227806481916393E-3</v>
-      </c>
-      <c r="N34" s="18">
-        <f>MAX(B34:J34)</f>
-        <v>0.5811540028948442</v>
-      </c>
-      <c r="P34" s="33">
-        <f>L34*100</f>
-        <v>20.58600597913038</v>
-      </c>
-      <c r="Q34" s="33">
-        <f>M34*100</f>
-        <v>0.35227806481916396</v>
-      </c>
-      <c r="R34" s="33">
-        <f>N34*100</f>
-        <v>58.11540028948442</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
@@ -1864,63 +2705,39 @@
         <v>0.31944276926788084</v>
       </c>
       <c r="C35" s="18">
-        <f t="shared" ref="C35:J35" si="5">SUM(C24:C28)</f>
+        <f t="shared" ref="C35:J35" si="12">SUM(C24:C28)</f>
         <v>0.35464650581076718</v>
       </c>
       <c r="D35" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0.39316841500965505</v>
       </c>
       <c r="E35" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0.68891943581161841</v>
       </c>
       <c r="F35" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0.68062931218636513</v>
       </c>
       <c r="G35" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0.27307252474199151</v>
       </c>
       <c r="H35" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0.54796414271467475</v>
       </c>
       <c r="I35" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0.56734812492569719</v>
       </c>
       <c r="J35" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0.55622663215415591</v>
       </c>
-      <c r="L35" s="18">
-        <f t="shared" ref="L35:L36" si="6">AVERAGE(B35:J35)</f>
-        <v>0.48682420695808953</v>
-      </c>
-      <c r="M35" s="18">
-        <f t="shared" ref="M35:M36" si="7">MIN(B35:J35)</f>
-        <v>0.27307252474199151</v>
-      </c>
-      <c r="N35" s="18">
-        <f t="shared" ref="N35:N36" si="8">MAX(B35:J35)</f>
-        <v>0.68891943581161841</v>
-      </c>
-      <c r="P35" s="33">
-        <f t="shared" ref="P35:P36" si="9">L35*100</f>
-        <v>48.68242069580895</v>
-      </c>
-      <c r="Q35" s="33">
-        <f t="shared" ref="Q35:Q36" si="10">M35*100</f>
-        <v>27.307252474199149</v>
-      </c>
-      <c r="R35" s="33">
-        <f t="shared" ref="R35:R36" si="11">N35*100</f>
-        <v>68.89194358116184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
@@ -1929,63 +2746,39 @@
         <v>0.27851485546576604</v>
       </c>
       <c r="C36" s="18">
-        <f t="shared" ref="C36:J36" si="12">C29</f>
+        <f t="shared" ref="C36:J36" si="13">C29</f>
         <v>6.4199491294388789E-2</v>
       </c>
       <c r="D36" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.60330880434215328</v>
       </c>
       <c r="E36" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.22113315802055941</v>
       </c>
       <c r="F36" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.1845362795177472</v>
       </c>
       <c r="G36" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.7198190058025441</v>
       </c>
       <c r="H36" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.41098566601670061</v>
       </c>
       <c r="I36" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.10069965787654496</v>
       </c>
       <c r="J36" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.18264468091905539</v>
       </c>
-      <c r="L36" s="18">
-        <f t="shared" si="6"/>
-        <v>0.30731573325060663</v>
-      </c>
-      <c r="M36" s="18">
-        <f t="shared" si="7"/>
-        <v>6.4199491294388789E-2</v>
-      </c>
-      <c r="N36" s="18">
-        <f t="shared" si="8"/>
-        <v>0.7198190058025441</v>
-      </c>
-      <c r="P36" s="33">
-        <f t="shared" si="9"/>
-        <v>30.731573325060662</v>
-      </c>
-      <c r="Q36" s="33">
-        <f t="shared" si="10"/>
-        <v>6.4199491294388791</v>
-      </c>
-      <c r="R36" s="33">
-        <f t="shared" si="11"/>
-        <v>71.981900580254404</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
@@ -1994,48 +2787,147 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="C37" s="18">
-        <f t="shared" ref="C37:J37" si="13">SUM(C34:C36)</f>
+        <f t="shared" ref="C37:J37" si="14">SUM(C34:C36)</f>
         <v>1.0000000000000002</v>
       </c>
       <c r="D37" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E37" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F37" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="G37" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="H37" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="I37" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="J37" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="P37">
-        <f>SUM(P34:P36)</f>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="18">
+        <f>AVERAGE(B34:J34)</f>
+        <v>0.20586005979130381</v>
+      </c>
+      <c r="D40" s="18">
+        <f>MIN(B34:J34)</f>
+        <v>3.5227806481916393E-3</v>
+      </c>
+      <c r="E40" s="18">
+        <f>MAX(B34:J34)</f>
+        <v>0.5811540028948442</v>
+      </c>
+      <c r="G40" s="30">
+        <f>C40*100</f>
+        <v>20.58600597913038</v>
+      </c>
+      <c r="H40" s="30">
+        <f>D40*100</f>
+        <v>0.35227806481916396</v>
+      </c>
+      <c r="I40" s="30">
+        <f>E40*100</f>
+        <v>58.11540028948442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="18">
+        <f>AVERAGE(B35:J35)</f>
+        <v>0.48682420695808953</v>
+      </c>
+      <c r="D41" s="18">
+        <f>MIN(B35:J35)</f>
+        <v>0.27307252474199151</v>
+      </c>
+      <c r="E41" s="18">
+        <f>MAX(B35:J35)</f>
+        <v>0.68891943581161841</v>
+      </c>
+      <c r="G41" s="30">
+        <f t="shared" ref="G41:G42" si="15">C41*100</f>
+        <v>48.68242069580895</v>
+      </c>
+      <c r="H41" s="30">
+        <f t="shared" ref="H41:H42" si="16">D41*100</f>
+        <v>27.307252474199149</v>
+      </c>
+      <c r="I41" s="30">
+        <f t="shared" ref="I41:I42" si="17">E41*100</f>
+        <v>68.89194358116184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="18">
+        <f>AVERAGE(B36:J36)</f>
+        <v>0.30731573325060663</v>
+      </c>
+      <c r="D42" s="18">
+        <f>MIN(B36:J36)</f>
+        <v>6.4199491294388789E-2</v>
+      </c>
+      <c r="E42" s="18">
+        <f>MAX(B36:J36)</f>
+        <v>0.7198190058025441</v>
+      </c>
+      <c r="G42" s="30">
+        <f t="shared" si="15"/>
+        <v>30.731573325060662</v>
+      </c>
+      <c r="H42" s="30">
+        <f t="shared" si="16"/>
+        <v>6.4199491294388791</v>
+      </c>
+      <c r="I42" s="30">
+        <f t="shared" si="17"/>
+        <v>71.981900580254404</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <f>SUM(G40:G42)</f>
         <v>100</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A17:J17"/>
     <mergeCell ref="A32:J32"/>
-    <mergeCell ref="P32:R32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2049,12 +2941,12 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2068,7 +2960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>11.2</v>
       </c>
@@ -2080,7 +2972,7 @@
         <v>24.492999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -2092,7 +2984,7 @@
         <v>10.259</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5.6</v>
       </c>
@@ -2104,7 +2996,7 @@
         <v>17.543800000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2116,7 +3008,7 @@
         <v>16.167000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2.8</v>
       </c>
@@ -2128,7 +3020,7 @@
         <v>14.247999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -2140,7 +3032,7 @@
         <v>13.518000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -2149,7 +3041,7 @@
         <v>0.56200000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -2158,7 +3050,7 @@
         <v>0.70120000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.71</v>
       </c>
@@ -2166,7 +3058,7 @@
         <v>0.84699999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.5</v>
       </c>
@@ -2175,7 +3067,7 @@
         <v>1.0680000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.25</v>
       </c>
@@ -2186,7 +3078,7 @@
         <v>9.1370000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2198,7 +3090,7 @@
         <v>1.9748000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2214,7 +3106,7 @@
         <v>107.34060000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2228,12 +3120,12 @@
         <v>120.92940000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -2244,7 +3136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>11.2</v>
       </c>
@@ -2258,7 +3150,7 @@
         <v>0.22818020394892516</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>8</v>
       </c>
@@ -2272,7 +3164,7 @@
         <v>9.5574274785123245E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>5.6</v>
       </c>
@@ -2286,7 +3178,7 @@
         <v>0.1634404875694751</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>4</v>
       </c>
@@ -2300,7 +3192,7 @@
         <v>0.1506140267522261</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>2.8</v>
       </c>
@@ -2314,7 +3206,7 @@
         <v>0.13273635511633061</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>2</v>
       </c>
@@ -2328,7 +3220,7 @@
         <v>0.1259355733059066</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>1.4</v>
       </c>
@@ -2342,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>1</v>
       </c>
@@ -2356,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>0.71</v>
       </c>
@@ -2370,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>0.5</v>
       </c>
@@ -2384,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>0.25</v>
       </c>
@@ -2398,7 +3290,7 @@
         <v>8.5121566303896196E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +3304,7 @@
         <v>1.8397512218116911E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -2425,7 +3317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>7</v>
       </c>
@@ -2442,7 +3334,7 @@
         <v>0.62810951606671472</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>8</v>
       </c>
@@ -2459,7 +3351,7 @@
         <v>0.31008002914086819</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>9</v>
       </c>
@@ -2476,7 +3368,7 @@
         <v>6.1810454792416966E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <f>SUM(C34:C36)</f>
         <v>1</v>
@@ -2486,12 +3378,12 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -2502,7 +3394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>11.2</v>
       </c>
@@ -2512,7 +3404,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>8</v>
       </c>
@@ -2522,7 +3414,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>5.6</v>
       </c>
@@ -2532,7 +3424,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>4</v>
       </c>
@@ -2542,7 +3434,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>2.8</v>
       </c>
@@ -2552,7 +3444,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>2</v>
       </c>
@@ -2562,7 +3454,7 @@
         <v>0.35973811065544281</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>1.4</v>
       </c>
@@ -2572,7 +3464,7 @@
         <v>0.41028131520253253</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>1</v>
       </c>
@@ -2582,7 +3474,7 @@
         <v>0.47334340600043168</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>0.71</v>
       </c>
@@ -2592,7 +3484,7 @@
         <v>0.54951795093172173</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>0.5</v>
       </c>
@@ -2602,7 +3494,7 @@
         <v>0.64556802647672495</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>0.25</v>
       </c>
@@ -2612,7 +3504,7 @@
         <v>0.89477660263328296</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
@@ -2635,12 +3527,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2654,7 +3546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>11.2</v>
       </c>
@@ -2668,7 +3560,7 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -2680,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5.6</v>
       </c>
@@ -2692,7 +3584,7 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2704,7 +3596,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2.8</v>
       </c>
@@ -2716,7 +3608,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -2728,7 +3620,7 @@
         <v>0.50700000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -2740,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -2752,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.71</v>
       </c>
@@ -2763,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.5</v>
       </c>
@@ -2775,7 +3667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.25</v>
       </c>
@@ -2786,7 +3678,7 @@
         <v>9.1370000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2798,7 +3690,7 @@
         <v>1.9748000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>